<commit_message>
Added extra bytes to handle button presses
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="80">
   <si>
     <t>1st</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Speed</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>41 H</t>
   </si>
   <si>
@@ -187,6 +184,78 @@
   </si>
   <si>
     <t>4C H</t>
+  </si>
+  <si>
+    <t>Value 1</t>
+  </si>
+  <si>
+    <t>Value 2</t>
+  </si>
+  <si>
+    <t>7th</t>
+  </si>
+  <si>
+    <t>8th</t>
+  </si>
+  <si>
+    <t>Value 3</t>
+  </si>
+  <si>
+    <t>Value 4</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>11th</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>Value 5</t>
+  </si>
+  <si>
+    <t>Value 6</t>
+  </si>
+  <si>
+    <t>Value 7</t>
+  </si>
+  <si>
+    <t>Value 8</t>
+  </si>
+  <si>
+    <t>6th Byte</t>
+  </si>
+  <si>
+    <t>8th Byte</t>
+  </si>
+  <si>
+    <t>9th Byte</t>
+  </si>
+  <si>
+    <t>10th Byte</t>
+  </si>
+  <si>
+    <t>11th Byte</t>
+  </si>
+  <si>
+    <t>12th Byte</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>23 H</t>
+  </si>
+  <si>
+    <t>13th Byte</t>
+  </si>
+  <si>
+    <t>13th</t>
   </si>
 </sst>
 </file>
@@ -294,16 +363,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -609,19 +676,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T34"/>
+  <dimension ref="B2:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="13" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="2"/>
+    <col min="2" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="7.140625" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="2" customWidth="1"/>
+    <col min="21" max="27" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,8 +710,31 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -655,43 +748,95 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="2:34" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA5" s="8"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -711,26 +856,69 @@
         <v>12</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -742,7 +930,7 @@
         <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>22</v>
@@ -751,17 +939,60 @@
         <v>15</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -774,17 +1005,60 @@
         <v>16</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -797,9 +1071,24 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="3" t="s">
@@ -815,26 +1104,69 @@
         <v>12</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -846,24 +1178,67 @@
         <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -876,9 +1251,24 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+    </row>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="3" t="s">
@@ -894,26 +1284,69 @@
         <v>12</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>56</v>
+        <v>35</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -925,27 +1358,125 @@
         <v>14</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="AA14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="J15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -953,7 +1484,7 @@
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S18" s="2"/>
     </row>
@@ -962,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -970,15 +1501,15 @@
         <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -986,7 +1517,7 @@
         <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -994,90 +1525,97 @@
         <v>255</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>1</v>
+      <c r="B27" t="s">
+        <v>56</v>
       </c>
       <c r="C27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>128</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="J14:K14"/>
+  <mergeCells count="14">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updates to work with android software
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="84">
   <si>
     <t>1st</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>13th</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>LED's</t>
   </si>
 </sst>
 </file>
@@ -352,7 +364,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,13 +376,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -676,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AH34"/>
+  <dimension ref="B2:AH59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,43 +885,43 @@
       <c r="L6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Y6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z6" s="3" t="s">
@@ -944,43 +959,43 @@
       <c r="L7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="S7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U7" s="9" t="s">
+      <c r="U7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z7" s="3" t="s">
@@ -1010,43 +1025,43 @@
       <c r="L8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U8" s="9" t="s">
+      <c r="U8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="Y8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z8" s="3" t="s">
@@ -1118,43 +1133,43 @@
       <c r="L10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U10" s="9" t="s">
+      <c r="U10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W10" s="9" t="s">
+      <c r="W10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y10" s="9" t="s">
+      <c r="Y10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z10" s="3" t="s">
@@ -1183,50 +1198,50 @@
       <c r="I11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="7"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U11" s="9" t="s">
+      <c r="U11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W11" s="9" t="s">
+      <c r="W11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y11" s="9" t="s">
+      <c r="Y11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z11" s="3" t="s">
@@ -1292,49 +1307,49 @@
       <c r="J13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>34</v>
+      <c r="K13" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="S13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="T13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U13" s="9" t="s">
+      <c r="U13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="W13" s="9" t="s">
+      <c r="W13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="X13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Y13" s="9" t="s">
+      <c r="Y13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Z13" s="3" t="s">
@@ -1581,7 +1596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>68</v>
       </c>
@@ -1589,7 +1604,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>69</v>
       </c>
@@ -1597,19 +1612,1284 @@
         <v>50</v>
       </c>
     </row>
+    <row r="38" spans="2:27" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA38" s="8"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3">
+        <v>30</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="3">
+        <v>52</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="3">
+        <v>41</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="3">
+        <v>43</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39" s="6">
+        <v>23</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N39" s="6">
+        <v>23</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P39" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R39" s="6">
+        <v>23</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T39" s="6">
+        <v>23</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V39" s="6">
+        <v>23</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X39" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="3">
+        <v>57</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="3">
+        <v>41</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="3">
+        <v>30</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" s="6">
+        <v>23</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N40" s="6">
+        <v>23</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P40" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R40" s="6">
+        <v>23</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T40" s="6">
+        <v>23</v>
+      </c>
+      <c r="U40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V40" s="6">
+        <v>23</v>
+      </c>
+      <c r="W40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X40" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="3">
+        <v>31</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L41" s="6">
+        <v>23</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N41" s="6">
+        <v>23</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P41" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R41" s="6">
+        <v>23</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T41" s="6">
+        <v>23</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V41" s="6">
+        <v>23</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X41" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="3">
+        <v>31</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="3">
+        <v>52</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="3">
+        <v>41</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="3">
+        <v>43</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" s="6">
+        <v>23</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N43" s="6">
+        <v>23</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P43" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R43" s="6">
+        <v>23</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T43" s="6">
+        <v>23</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V43" s="6">
+        <v>23</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X43" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="3">
+        <v>57</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="3">
+        <v>41</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K44" s="9"/>
+      <c r="L44" s="6">
+        <v>23</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N44" s="6">
+        <v>23</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P44" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R44" s="6">
+        <v>23</v>
+      </c>
+      <c r="S44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T44" s="6">
+        <v>23</v>
+      </c>
+      <c r="U44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V44" s="6">
+        <v>23</v>
+      </c>
+      <c r="W44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X44" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="3">
+        <v>32</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="3">
+        <v>52</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="3">
+        <v>41</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L46" s="6">
+        <v>23</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N46" s="6">
+        <v>23</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P46" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R46" s="6">
+        <v>23</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T46" s="6">
+        <v>23</v>
+      </c>
+      <c r="U46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V46" s="6">
+        <v>23</v>
+      </c>
+      <c r="W46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X46" s="6">
+        <v>23</v>
+      </c>
+      <c r="Y46" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z46" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="3">
+        <v>57</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="3">
+        <v>41</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J47" s="3">
+        <v>30</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="3">
+        <v>30</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" s="3">
+        <v>30</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P47" s="3">
+        <v>30</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R47" s="3">
+        <v>30</v>
+      </c>
+      <c r="S47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T47" s="3">
+        <v>30</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V47" s="3">
+        <v>30</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="X47" s="3">
+        <v>30</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z47" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="J48" s="3">
+        <v>31</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L48" s="3">
+        <v>31</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N48" s="3">
+        <v>31</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P48" s="3">
+        <v>31</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R48" s="3">
+        <v>31</v>
+      </c>
+      <c r="S48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T48" s="3">
+        <v>31</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V48" s="3">
+        <v>31</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X48" s="3">
+        <v>31</v>
+      </c>
+      <c r="Y48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z48" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA48" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:27" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="8"/>
+      <c r="X49" s="8"/>
+      <c r="Y49" s="8"/>
+      <c r="Z49" s="8"/>
+      <c r="AA49" s="8"/>
+    </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B50" s="3">
+        <f>HEX2DEC(B39)</f>
+        <v>27</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="3">
+        <f>HEX2DEC(D39)</f>
+        <v>48</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="3">
+        <f>HEX2DEC(F39)</f>
+        <v>82</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="3">
+        <f>HEX2DEC(H39)</f>
+        <v>65</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="3">
+        <f>HEX2DEC(J39)</f>
+        <v>67</v>
+      </c>
+      <c r="K50" s="4"/>
+      <c r="L50" s="3">
+        <f>HEX2DEC(L39)</f>
+        <v>35</v>
+      </c>
+      <c r="M50" s="7"/>
+      <c r="N50" s="3">
+        <f>HEX2DEC(N39)</f>
+        <v>35</v>
+      </c>
+      <c r="O50" s="7"/>
+      <c r="P50" s="3">
+        <f>HEX2DEC(P39)</f>
+        <v>35</v>
+      </c>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="3">
+        <f>HEX2DEC(R39)</f>
+        <v>35</v>
+      </c>
+      <c r="S50" s="7"/>
+      <c r="T50" s="3">
+        <f>HEX2DEC(T39)</f>
+        <v>35</v>
+      </c>
+      <c r="U50" s="7"/>
+      <c r="V50" s="3">
+        <f>HEX2DEC(V39)</f>
+        <v>35</v>
+      </c>
+      <c r="W50" s="7"/>
+      <c r="X50" s="3">
+        <f>HEX2DEC(X39)</f>
+        <v>35</v>
+      </c>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="3">
+        <f>HEX2DEC(Z39)</f>
+        <v>10</v>
+      </c>
+      <c r="AA50" s="4"/>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="3">
+        <f>HEX2DEC(F40)</f>
+        <v>87</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="3">
+        <f>HEX2DEC(H40)</f>
+        <v>65</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="3">
+        <f>HEX2DEC(J40)</f>
+        <v>48</v>
+      </c>
+      <c r="K51" s="4"/>
+      <c r="L51" s="3">
+        <f>HEX2DEC(L40)</f>
+        <v>35</v>
+      </c>
+      <c r="M51" s="7"/>
+      <c r="N51" s="3">
+        <f>HEX2DEC(N40)</f>
+        <v>35</v>
+      </c>
+      <c r="O51" s="7"/>
+      <c r="P51" s="3">
+        <f>HEX2DEC(P40)</f>
+        <v>35</v>
+      </c>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="3">
+        <f>HEX2DEC(R40)</f>
+        <v>35</v>
+      </c>
+      <c r="S51" s="7"/>
+      <c r="T51" s="3">
+        <f>HEX2DEC(T40)</f>
+        <v>35</v>
+      </c>
+      <c r="U51" s="7"/>
+      <c r="V51" s="3">
+        <f>HEX2DEC(V40)</f>
+        <v>35</v>
+      </c>
+      <c r="W51" s="7"/>
+      <c r="X51" s="3">
+        <f>HEX2DEC(X40)</f>
+        <v>35</v>
+      </c>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="3">
+        <f>HEX2DEC(Z40)</f>
+        <v>10</v>
+      </c>
+      <c r="AA51" s="4"/>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="3">
+        <f>HEX2DEC(J41)</f>
+        <v>49</v>
+      </c>
+      <c r="K52" s="4"/>
+      <c r="L52" s="3">
+        <f>HEX2DEC(L41)</f>
+        <v>35</v>
+      </c>
+      <c r="M52" s="7"/>
+      <c r="N52" s="3">
+        <f>HEX2DEC(N41)</f>
+        <v>35</v>
+      </c>
+      <c r="O52" s="7"/>
+      <c r="P52" s="3">
+        <f>HEX2DEC(P41)</f>
+        <v>35</v>
+      </c>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="3">
+        <f>HEX2DEC(R41)</f>
+        <v>35</v>
+      </c>
+      <c r="S52" s="7"/>
+      <c r="T52" s="3">
+        <f>HEX2DEC(T41)</f>
+        <v>35</v>
+      </c>
+      <c r="U52" s="7"/>
+      <c r="V52" s="3">
+        <f>HEX2DEC(V41)</f>
+        <v>35</v>
+      </c>
+      <c r="W52" s="7"/>
+      <c r="X52" s="3">
+        <f>HEX2DEC(X41)</f>
+        <v>35</v>
+      </c>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="3">
+        <f>HEX2DEC(Z41)</f>
+        <v>10</v>
+      </c>
+      <c r="AA52" s="4"/>
+    </row>
+    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+    </row>
+    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="3">
+        <f>HEX2DEC(D43)</f>
+        <v>49</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="3">
+        <f>HEX2DEC(F43)</f>
+        <v>82</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="3">
+        <f>HEX2DEC(H43)</f>
+        <v>65</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="3">
+        <f>HEX2DEC(J43)</f>
+        <v>67</v>
+      </c>
+      <c r="K54" s="4"/>
+      <c r="L54" s="3">
+        <f>HEX2DEC(L43)</f>
+        <v>35</v>
+      </c>
+      <c r="M54" s="7"/>
+      <c r="N54" s="3">
+        <f>HEX2DEC(N43)</f>
+        <v>35</v>
+      </c>
+      <c r="O54" s="7"/>
+      <c r="P54" s="3">
+        <f>HEX2DEC(P43)</f>
+        <v>35</v>
+      </c>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="3">
+        <f>HEX2DEC(R43)</f>
+        <v>35</v>
+      </c>
+      <c r="S54" s="7"/>
+      <c r="T54" s="3">
+        <f>HEX2DEC(T43)</f>
+        <v>35</v>
+      </c>
+      <c r="U54" s="7"/>
+      <c r="V54" s="3">
+        <f>HEX2DEC(V43)</f>
+        <v>35</v>
+      </c>
+      <c r="W54" s="7"/>
+      <c r="X54" s="3">
+        <f>HEX2DEC(X43)</f>
+        <v>35</v>
+      </c>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="3">
+        <f>HEX2DEC(Z43)</f>
+        <v>10</v>
+      </c>
+      <c r="AA54" s="4"/>
+    </row>
+    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="3">
+        <f>HEX2DEC(F44)</f>
+        <v>87</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="3">
+        <f>HEX2DEC(H44)</f>
+        <v>65</v>
+      </c>
+      <c r="I55" s="4"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="3">
+        <f>HEX2DEC(L44)</f>
+        <v>35</v>
+      </c>
+      <c r="M55" s="7"/>
+      <c r="N55" s="3">
+        <f>HEX2DEC(N44)</f>
+        <v>35</v>
+      </c>
+      <c r="O55" s="7"/>
+      <c r="P55" s="3">
+        <f>HEX2DEC(P44)</f>
+        <v>35</v>
+      </c>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="3">
+        <f>HEX2DEC(R44)</f>
+        <v>35</v>
+      </c>
+      <c r="S55" s="7"/>
+      <c r="T55" s="3">
+        <f>HEX2DEC(T44)</f>
+        <v>35</v>
+      </c>
+      <c r="U55" s="7"/>
+      <c r="V55" s="3">
+        <f>HEX2DEC(V44)</f>
+        <v>35</v>
+      </c>
+      <c r="W55" s="7"/>
+      <c r="X55" s="3">
+        <f>HEX2DEC(X44)</f>
+        <v>35</v>
+      </c>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="3">
+        <f>HEX2DEC(Z44)</f>
+        <v>10</v>
+      </c>
+      <c r="AA55" s="4"/>
+    </row>
+    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+    </row>
+    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="3">
+        <f>HEX2DEC(D46)</f>
+        <v>50</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="3">
+        <f>HEX2DEC(F46)</f>
+        <v>82</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="3">
+        <f>HEX2DEC(H46)</f>
+        <v>65</v>
+      </c>
+      <c r="I57" s="4"/>
+      <c r="J57" s="3">
+        <f>HEX2DEC(J46)</f>
+        <v>76</v>
+      </c>
+      <c r="K57" s="4"/>
+      <c r="L57" s="3">
+        <f>HEX2DEC(L46)</f>
+        <v>35</v>
+      </c>
+      <c r="M57" s="7"/>
+      <c r="N57" s="3">
+        <f>HEX2DEC(N46)</f>
+        <v>35</v>
+      </c>
+      <c r="O57" s="7"/>
+      <c r="P57" s="3">
+        <f>HEX2DEC(P46)</f>
+        <v>35</v>
+      </c>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="3">
+        <f>HEX2DEC(R46)</f>
+        <v>35</v>
+      </c>
+      <c r="S57" s="7"/>
+      <c r="T57" s="3">
+        <f>HEX2DEC(T46)</f>
+        <v>35</v>
+      </c>
+      <c r="U57" s="7"/>
+      <c r="V57" s="3">
+        <f>HEX2DEC(V46)</f>
+        <v>35</v>
+      </c>
+      <c r="W57" s="7"/>
+      <c r="X57" s="3">
+        <f>HEX2DEC(X46)</f>
+        <v>35</v>
+      </c>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="3">
+        <f>HEX2DEC(Z46)</f>
+        <v>10</v>
+      </c>
+      <c r="AA57" s="4"/>
+    </row>
+    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="3">
+        <f>HEX2DEC(F47)</f>
+        <v>87</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="3">
+        <f>HEX2DEC(H47)</f>
+        <v>65</v>
+      </c>
+      <c r="I58" s="4"/>
+      <c r="J58" s="3">
+        <f>HEX2DEC(J47)</f>
+        <v>48</v>
+      </c>
+      <c r="K58" s="4"/>
+      <c r="L58" s="3">
+        <f>HEX2DEC(L47)</f>
+        <v>48</v>
+      </c>
+      <c r="M58" s="4"/>
+      <c r="N58" s="3">
+        <f>HEX2DEC(N47)</f>
+        <v>48</v>
+      </c>
+      <c r="O58" s="4"/>
+      <c r="P58" s="3">
+        <f>HEX2DEC(P47)</f>
+        <v>48</v>
+      </c>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="3">
+        <f>HEX2DEC(R47)</f>
+        <v>48</v>
+      </c>
+      <c r="S58" s="4"/>
+      <c r="T58" s="3">
+        <f>HEX2DEC(T47)</f>
+        <v>48</v>
+      </c>
+      <c r="U58" s="4"/>
+      <c r="V58" s="3">
+        <f>HEX2DEC(V47)</f>
+        <v>48</v>
+      </c>
+      <c r="W58" s="4"/>
+      <c r="X58" s="3">
+        <f>HEX2DEC(X47)</f>
+        <v>48</v>
+      </c>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="3">
+        <f>HEX2DEC(Z47)</f>
+        <v>10</v>
+      </c>
+      <c r="AA58" s="4"/>
+    </row>
+    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="J59" s="3">
+        <f>HEX2DEC(J48)</f>
+        <v>49</v>
+      </c>
+      <c r="K59" s="4"/>
+      <c r="L59" s="3">
+        <f>HEX2DEC(L48)</f>
+        <v>49</v>
+      </c>
+      <c r="M59" s="4"/>
+      <c r="N59" s="3">
+        <f>HEX2DEC(N48)</f>
+        <v>49</v>
+      </c>
+      <c r="O59" s="4"/>
+      <c r="P59" s="3">
+        <f>HEX2DEC(P48)</f>
+        <v>49</v>
+      </c>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="3">
+        <f>HEX2DEC(R48)</f>
+        <v>49</v>
+      </c>
+      <c r="S59" s="4"/>
+      <c r="T59" s="3">
+        <f>HEX2DEC(T48)</f>
+        <v>49</v>
+      </c>
+      <c r="U59" s="4"/>
+      <c r="V59" s="3">
+        <f>HEX2DEC(V48)</f>
+        <v>49</v>
+      </c>
+      <c r="W59" s="4"/>
+      <c r="X59" s="3">
+        <f>HEX2DEC(X48)</f>
+        <v>49</v>
+      </c>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="3">
+        <f>HEX2DEC(Z48)</f>
+        <v>10</v>
+      </c>
+      <c r="AA59" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="42">
+    <mergeCell ref="Z49:AA49"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="V49:W49"/>
+    <mergeCell ref="X49:Y49"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="X5:Y5"/>

</xml_diff>

<commit_message>
got serial communication working
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="85">
   <si>
     <t>1st</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>LED's</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x30,</t>
   </si>
 </sst>
 </file>
@@ -693,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
@@ -1595,6 +1598,9 @@
       <c r="C32" t="s">
         <v>53</v>
       </c>
+      <c r="S32" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -2851,17 +2857,38 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
     <mergeCell ref="Z49:AA49"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="V38:W38"/>
     <mergeCell ref="X38:Y38"/>
     <mergeCell ref="Z38:AA38"/>
     <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
     <mergeCell ref="L49:M49"/>
     <mergeCell ref="N49:O49"/>
     <mergeCell ref="P49:Q49"/>
@@ -2872,27 +2899,6 @@
     <mergeCell ref="L38:M38"/>
     <mergeCell ref="N38:O38"/>
     <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added security code for authentication
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="93">
   <si>
     <t>1st</t>
   </si>
@@ -265,6 +265,36 @@
   </si>
   <si>
     <t>Power State</t>
+  </si>
+  <si>
+    <t>Code 1</t>
+  </si>
+  <si>
+    <t>Code 2</t>
+  </si>
+  <si>
+    <t>Code 3</t>
+  </si>
+  <si>
+    <t>Code 4</t>
+  </si>
+  <si>
+    <t>Code 5</t>
+  </si>
+  <si>
+    <t>14th</t>
+  </si>
+  <si>
+    <t>15th</t>
+  </si>
+  <si>
+    <t>16th</t>
+  </si>
+  <si>
+    <t>17th</t>
+  </si>
+  <si>
+    <t>18th</t>
   </si>
 </sst>
 </file>
@@ -374,10 +404,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,22 +715,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AH38"/>
+  <dimension ref="B2:AR38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="7.140625" customWidth="1"/>
-    <col min="20" max="20" width="7.140625" style="2" customWidth="1"/>
-    <col min="21" max="27" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,172 +783,206 @@
       <c r="N2" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="T2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AE2" s="2"/>
+    </row>
+    <row r="3" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="T3"/>
-      <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AE3" s="2"/>
+    </row>
+    <row r="4" spans="2:44" x14ac:dyDescent="0.25">
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="2:34" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="O5" s="9"/>
+      <c r="P5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
+      <c r="S5" s="9"/>
+      <c r="T5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="U5" s="9"/>
+      <c r="V5" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8" t="s">
+      <c r="W5" s="9"/>
+      <c r="X5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8" t="s">
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8" t="s">
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8" t="s">
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8" t="s">
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8" t="s">
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8" t="s">
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="AA5" s="8"/>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
-    </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AK5" s="9"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+    </row>
+    <row r="6" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V6" s="6" t="s">
         <v>77</v>
       </c>
@@ -918,16 +995,46 @@
       <c r="Y6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AK6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -954,62 +1061,52 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+    </row>
+    <row r="8" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="U8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U8" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V8" s="6" t="s">
         <v>77</v>
       </c>
@@ -1022,16 +1119,46 @@
       <c r="Y8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z8" s="3" t="s">
+      <c r="Z8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
-    </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1040,42 +1167,22 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="U9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V9" s="6" t="s">
         <v>77</v>
       </c>
@@ -1088,16 +1195,46 @@
       <c r="Y9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z9" s="3" t="s">
+      <c r="Z9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="4" t="s">
+      <c r="AK9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+    </row>
+    <row r="10" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1124,66 +1261,56 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2"/>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+    </row>
+    <row r="11" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="T11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="U11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U11" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V11" s="6" t="s">
         <v>77</v>
       </c>
@@ -1196,16 +1323,46 @@
       <c r="Y11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z11" s="3" t="s">
+      <c r="Z11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA11" s="4" t="s">
+      <c r="AK11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+    </row>
+    <row r="12" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1232,60 +1389,50 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+    </row>
+    <row r="13" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="R13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="T13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="U13" s="8"/>
       <c r="V13" s="6" t="s">
         <v>77</v>
       </c>
@@ -1298,16 +1445,46 @@
       <c r="Y13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z13" s="3" t="s">
+      <c r="Z13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA13" s="4" t="s">
+      <c r="AK13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+    </row>
+    <row r="14" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1334,66 +1511,56 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+    </row>
+    <row r="15" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="T15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="U15" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V15" s="6" t="s">
         <v>77</v>
       </c>
@@ -1406,16 +1573,46 @@
       <c r="Y15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z15" s="3" t="s">
+      <c r="Z15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA15" s="4" t="s">
+      <c r="AK15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+    </row>
+    <row r="16" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1442,55 +1639,45 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+    </row>
+    <row r="17" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="S17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>15</v>
@@ -1511,15 +1698,45 @@
         <v>32</v>
       </c>
       <c r="Z17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA17" s="4" t="s">
+      <c r="AK17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+    </row>
+    <row r="18" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1528,36 +1745,16 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S18" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
       <c r="T18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1577,13 +1774,43 @@
         <v>33</v>
       </c>
       <c r="Z18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA18" s="4" t="s">
+      <c r="AK18" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1610,56 +1837,46 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+    </row>
+    <row r="20" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="S20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="T20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="U20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S20" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V20" s="6" t="s">
         <v>77</v>
       </c>
@@ -1672,14 +1889,44 @@
       <c r="Y20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z20" s="3" t="s">
+      <c r="Z20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA20" s="4" t="s">
+      <c r="AK20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1688,42 +1935,22 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="U21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="P21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="S21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="T21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="U21" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="V21" s="6" t="s">
         <v>77</v>
       </c>
@@ -1736,20 +1963,50 @@
       <c r="Y21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="Z21" s="3" t="s">
+      <c r="Z21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA21" s="4" t="s">
+      <c r="AK21" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>37</v>
       </c>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>0</v>
       </c>
@@ -1757,7 +2014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>126</v>
       </c>
@@ -1765,7 +2022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>45</v>
       </c>
@@ -1773,7 +2030,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>129</v>
       </c>
@@ -1781,7 +2038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>255</v>
       </c>
@@ -1789,12 +2046,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>56</v>
       </c>
@@ -1802,7 +2059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>57</v>
       </c>
@@ -1859,21 +2116,26 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L5:M5"/>
+  <mergeCells count="19">
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="N5:O5"/>
+    <mergeCell ref="AJ5:AK5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="T13:U13"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to Comms and PC software
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="117">
   <si>
     <t>1st</t>
   </si>
@@ -322,6 +322,51 @@
   </si>
   <si>
     <t>Comms Nano</t>
+  </si>
+  <si>
+    <t>33 H</t>
+  </si>
+  <si>
+    <t>Lighting</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>34 H</t>
+  </si>
+  <si>
+    <t>35 H</t>
+  </si>
+  <si>
+    <t>36 H</t>
+  </si>
+  <si>
+    <t>Mode 1</t>
+  </si>
+  <si>
+    <t>Mode 2</t>
+  </si>
+  <si>
+    <t>Mode 3</t>
+  </si>
+  <si>
+    <t>Mode 4</t>
+  </si>
+  <si>
+    <t>Mode 5</t>
+  </si>
+  <si>
+    <t>Mode 6</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>50 H</t>
   </si>
 </sst>
 </file>
@@ -418,7 +463,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,6 +480,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -746,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AR47"/>
+  <dimension ref="B2:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,154 +940,154 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12" t="s">
+      <c r="M5" s="13"/>
+      <c r="N5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="13"/>
+      <c r="P5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12" t="s">
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12" t="s">
+      <c r="S5" s="13"/>
+      <c r="T5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12" t="s">
+      <c r="U5" s="13"/>
+      <c r="V5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12" t="s">
+      <c r="W5" s="13"/>
+      <c r="X5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12" t="s">
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12" t="s">
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12" t="s">
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12" t="s">
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12" t="s">
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12" t="s">
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="AK5" s="12"/>
+      <c r="AK5" s="13"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
     </row>
     <row r="6" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12" t="s">
+      <c r="K6" s="13"/>
+      <c r="L6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12" t="s">
+      <c r="O6" s="13"/>
+      <c r="P6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12" t="s">
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12" t="s">
+      <c r="S6" s="13"/>
+      <c r="T6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12" t="s">
+      <c r="U6" s="13"/>
+      <c r="V6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12" t="s">
+      <c r="W6" s="13"/>
+      <c r="X6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12" t="s">
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12" t="s">
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12" t="s">
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12" t="s">
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12" t="s">
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="AI6" s="12"/>
-      <c r="AJ6" s="12" t="s">
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AK6" s="12"/>
+      <c r="AK6" s="13"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
     </row>
@@ -1446,8 +1492,8 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="4"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="6" t="s">
         <v>99</v>
       </c>
@@ -1494,8 +1540,8 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="4"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="6" t="s">
         <v>48</v>
       </c>
@@ -1542,8 +1588,8 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="4"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="9"/>
       <c r="T15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1960,10 +2006,10 @@
       <c r="S22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="13" t="s">
+      <c r="T22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="U22" s="13"/>
+      <c r="U22" s="14"/>
       <c r="V22" s="6" t="s">
         <v>64</v>
       </c>
@@ -2156,24 +2202,60 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5"/>
-      <c r="AH25" s="5"/>
-      <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
-      <c r="AK25" s="5"/>
+      <c r="T25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK25" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
@@ -2190,72 +2272,28 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK26" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -2272,57 +2310,65 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
+      <c r="P27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="T27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AF27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AG27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AJ27" s="3" t="s">
         <v>33</v>
@@ -2350,24 +2396,60 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5"/>
-      <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
-      <c r="AK28" s="5"/>
+      <c r="T28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK28" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
@@ -2386,66 +2468,26 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
-      <c r="R29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH29" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK29" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
@@ -2464,13 +2506,17 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
+      <c r="R30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="T30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V30" s="6" t="s">
         <v>64</v>
@@ -2522,117 +2568,1051 @@
       </c>
     </row>
     <row r="31" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK31" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+    </row>
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="T33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK33" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="11"/>
+      <c r="AH34" s="10"/>
+      <c r="AI34" s="11"/>
+      <c r="AJ34" s="8"/>
+      <c r="AK34" s="9"/>
+    </row>
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="T35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK35" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK36" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="10"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="11"/>
+      <c r="AJ37" s="8"/>
+      <c r="AK37" s="9"/>
+    </row>
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U38" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK38" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK39" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="U40" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK40" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="V42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK42" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="V43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK43" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="12"/>
+      <c r="AD44" s="12"/>
+      <c r="AE44" s="12"/>
+      <c r="AF44" s="12"/>
+      <c r="AG44" s="12"/>
+      <c r="AH44" s="12"/>
+      <c r="AI44" s="12"/>
+      <c r="AJ44" s="12"/>
+      <c r="AK44" s="12"/>
+    </row>
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>31</v>
       </c>
-      <c r="S31" s="2"/>
-    </row>
-    <row r="32" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
+      <c r="S45" s="2"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="12"/>
+      <c r="AF45" s="12"/>
+      <c r="AG45" s="12"/>
+      <c r="AH45" s="12"/>
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="12"/>
+      <c r="AK45" s="12"/>
+    </row>
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
         <v>0</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
         <v>126</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C47" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C48" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
         <v>129</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
         <v>255</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>49</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C55" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>53</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>54</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>59</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>60</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>61</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C60" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>62</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C61" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started work on mega serial control
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="116">
   <si>
     <t>1st</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>Begin</t>
-  </si>
-  <si>
-    <t>Device IS</t>
   </si>
   <si>
     <t>R/W</t>
@@ -792,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AR61"/>
+  <dimension ref="B2:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,79 +934,98 @@
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="S4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4"/>
+      <c r="AE4" s="2"/>
     </row>
     <row r="5" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="13">
         <v>0</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="13">
         <v>2</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="13">
         <v>3</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="13">
         <v>4</v>
       </c>
       <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="13">
         <v>5</v>
       </c>
       <c r="M5" s="13"/>
-      <c r="N5" s="13" t="s">
-        <v>51</v>
+      <c r="N5" s="13">
+        <v>6</v>
       </c>
       <c r="O5" s="13"/>
-      <c r="P5" s="13" t="s">
-        <v>52</v>
+      <c r="P5" s="13">
+        <v>7</v>
       </c>
       <c r="Q5" s="13"/>
-      <c r="R5" s="13" t="s">
-        <v>55</v>
+      <c r="R5" s="13">
+        <v>8</v>
       </c>
       <c r="S5" s="13"/>
-      <c r="T5" s="13" t="s">
-        <v>56</v>
+      <c r="T5" s="13">
+        <v>9</v>
       </c>
       <c r="U5" s="13"/>
-      <c r="V5" s="13" t="s">
-        <v>57</v>
+      <c r="V5" s="13">
+        <v>10</v>
       </c>
       <c r="W5" s="13"/>
-      <c r="X5" s="13" t="s">
-        <v>58</v>
+      <c r="X5" s="13">
+        <v>11</v>
       </c>
       <c r="Y5" s="13"/>
-      <c r="Z5" s="13" t="s">
-        <v>65</v>
+      <c r="Z5" s="13">
+        <v>12</v>
       </c>
       <c r="AA5" s="13"/>
-      <c r="AB5" s="13" t="s">
-        <v>74</v>
+      <c r="AB5" s="13">
+        <v>13</v>
       </c>
       <c r="AC5" s="13"/>
-      <c r="AD5" s="13" t="s">
-        <v>75</v>
+      <c r="AD5" s="13">
+        <v>14</v>
       </c>
       <c r="AE5" s="13"/>
-      <c r="AF5" s="13" t="s">
-        <v>76</v>
+      <c r="AF5" s="13">
+        <v>15</v>
       </c>
       <c r="AG5" s="13"/>
-      <c r="AH5" s="13" t="s">
-        <v>77</v>
+      <c r="AH5" s="13">
+        <v>16</v>
       </c>
       <c r="AI5" s="13"/>
-      <c r="AJ5" s="13" t="s">
-        <v>78</v>
+      <c r="AJ5" s="13">
+        <v>17</v>
       </c>
       <c r="AK5" s="13"/>
       <c r="AQ5" s="2"/>
@@ -1017,209 +1033,245 @@
     </row>
     <row r="6" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="13"/>
       <c r="R6" s="13" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="S6" s="13"/>
       <c r="T6" s="13" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="U6" s="13"/>
       <c r="V6" s="13" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="W6" s="13"/>
       <c r="X6" s="13" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="Y6" s="13"/>
       <c r="Z6" s="13" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="AE6" s="13"/>
       <c r="AF6" s="13" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="AG6" s="13"/>
       <c r="AH6" s="13" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="AK6" s="13"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
     </row>
-    <row r="7" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK7" s="4" t="s">
+    <row r="7" spans="2:44" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="AK7" s="13"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
     </row>
     <row r="8" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
     </row>
@@ -1238,72 +1290,28 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK9" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
     </row>
@@ -1322,15 +1330,23 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+      <c r="P10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="T10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V10" s="6" t="s">
         <v>64</v>
@@ -1402,24 +1418,60 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="10"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="10"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="10"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="9"/>
+      <c r="T11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK11" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
     </row>
@@ -1440,38 +1492,26 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
-      <c r="R12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="V12" s="6"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="7"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="7"/>
-      <c r="AJ12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK12" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="9"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
     </row>
@@ -1492,13 +1532,17 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
+      <c r="R13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="T13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" s="7"/>
@@ -1543,10 +1587,10 @@
       <c r="R14" s="8"/>
       <c r="S14" s="9"/>
       <c r="T14" s="6" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V14" s="6"/>
       <c r="W14" s="7"/>
@@ -1591,10 +1635,10 @@
       <c r="R15" s="8"/>
       <c r="S15" s="9"/>
       <c r="T15" s="6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="V15" s="6"/>
       <c r="W15" s="7"/>
@@ -1636,26 +1680,34 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
-      <c r="AE16" s="5"/>
-      <c r="AF16" s="5"/>
-      <c r="AG16" s="5"/>
-      <c r="AH16" s="5"/>
-      <c r="AI16" s="5"/>
-      <c r="AJ16" s="5"/>
-      <c r="AK16" s="5"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="V16" s="6"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK16" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
     </row>
@@ -1676,66 +1728,26 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
-      <c r="R17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="U17" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="V17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK17" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
     </row>
@@ -1756,13 +1768,17 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="R18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="T18" s="6" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="V18" s="6" t="s">
         <v>64</v>
@@ -1834,24 +1850,60 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="5"/>
-      <c r="AG19" s="5"/>
-      <c r="AH19" s="5"/>
-      <c r="AI19" s="5"/>
-      <c r="AJ19" s="5"/>
-      <c r="AK19" s="5"/>
+      <c r="T19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK19" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
     </row>
@@ -1868,78 +1920,32 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK20" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
     </row>
     <row r="21" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
@@ -1954,30 +1960,78 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-      <c r="AG21" s="5"/>
-      <c r="AH21" s="5"/>
-      <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
-      <c r="AK21" s="5"/>
+      <c r="N21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK21" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
@@ -1994,70 +2048,28 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="U22" s="14"/>
-      <c r="V22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK22" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
     </row>
     <row r="23" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
@@ -2074,28 +2086,70 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AG23" s="5"/>
-      <c r="AH23" s="5"/>
-      <c r="AI23" s="5"/>
-      <c r="AJ23" s="5"/>
-      <c r="AK23" s="5"/>
+      <c r="P23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="U23" s="14"/>
+      <c r="V23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK23" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
@@ -2110,78 +2164,30 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-      <c r="N24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="U24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH24" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ24" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK24" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
     </row>
     <row r="25" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
@@ -2196,17 +2202,29 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
+      <c r="N25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="T25" s="6" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="V25" s="6" t="s">
         <v>64</v>
@@ -2276,24 +2294,60 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
-      <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
-      <c r="AK26" s="5"/>
+      <c r="T26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="V26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK26" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -2310,72 +2364,28 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK27" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
@@ -2392,57 +2402,65 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
+      <c r="P28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="T28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AF28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AG28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI28" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AJ28" s="3" t="s">
         <v>33</v>
@@ -2470,24 +2488,60 @@
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="5"/>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5"/>
+      <c r="T29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK29" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
@@ -2506,66 +2560,26 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
-      <c r="R30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK30" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
     </row>
     <row r="31" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
@@ -2584,13 +2598,17 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
+      <c r="R31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="T31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V31" s="6" t="s">
         <v>64</v>
@@ -2660,24 +2678,60 @@
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-      <c r="AG32" s="5"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
-      <c r="AJ32" s="5"/>
-      <c r="AK32" s="5"/>
+      <c r="T32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK32" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
@@ -2692,78 +2746,30 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S33" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="T33" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="U33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="V33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK33" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
     </row>
     <row r="34" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
@@ -2778,30 +2784,78 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="10"/>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="10"/>
-      <c r="AA34" s="11"/>
-      <c r="AB34" s="10"/>
-      <c r="AC34" s="11"/>
-      <c r="AD34" s="10"/>
-      <c r="AE34" s="11"/>
-      <c r="AF34" s="10"/>
-      <c r="AG34" s="11"/>
-      <c r="AH34" s="10"/>
-      <c r="AI34" s="11"/>
-      <c r="AJ34" s="8"/>
-      <c r="AK34" s="9"/>
+      <c r="N34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="T34" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK34" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
@@ -2818,72 +2872,28 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="T35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U35" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="V35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK35" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="10"/>
+      <c r="AI35" s="11"/>
+      <c r="AJ35" s="8"/>
+      <c r="AK35" s="9"/>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
@@ -2900,15 +2910,23 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U36" s="4" t="s">
-        <v>27</v>
+      <c r="P36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="T36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="U36" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="V36" s="6" t="s">
         <v>64</v>
@@ -2978,24 +2996,60 @@
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="10"/>
-      <c r="W37" s="11"/>
-      <c r="X37" s="10"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="10"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="10"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="10"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="11"/>
-      <c r="AH37" s="10"/>
-      <c r="AI37" s="11"/>
-      <c r="AJ37" s="8"/>
-      <c r="AK37" s="9"/>
+      <c r="T37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK37" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
@@ -3014,66 +3068,26 @@
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
-      <c r="R38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S38" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="T38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="U38" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="V38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ38" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK38" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="10"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="11"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="11"/>
+      <c r="AJ38" s="8"/>
+      <c r="AK38" s="9"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
@@ -3092,13 +3106,17 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
+      <c r="R39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S39" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="T39" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="V39" s="6" t="s">
         <v>64</v>
@@ -3169,10 +3187,10 @@
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="6" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V40" s="6" t="s">
         <v>64</v>
@@ -3243,10 +3261,10 @@
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>64</v>
@@ -3317,10 +3335,10 @@
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="V42" s="6" t="s">
         <v>64</v>
@@ -3391,10 +3409,10 @@
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V43" s="6" t="s">
         <v>64</v>
@@ -3446,48 +3464,98 @@
       </c>
     </row>
     <row r="44" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="12"/>
-      <c r="S44" s="12"/>
-      <c r="T44" s="12"/>
-      <c r="U44" s="12"/>
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-      <c r="X44" s="12"/>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
-      <c r="AA44" s="12"/>
-      <c r="AB44" s="12"/>
-      <c r="AC44" s="12"/>
-      <c r="AD44" s="12"/>
-      <c r="AE44" s="12"/>
-      <c r="AF44" s="12"/>
-      <c r="AG44" s="12"/>
-      <c r="AH44" s="12"/>
-      <c r="AI44" s="12"/>
-      <c r="AJ44" s="12"/>
-      <c r="AK44" s="12"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="U44" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="V44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK44" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>31</v>
-      </c>
-      <c r="S45" s="2"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
       <c r="T45" s="12"/>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
@@ -3508,153 +3576,195 @@
       <c r="AK45" s="12"/>
     </row>
     <row r="46" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B46" s="2">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="S46" s="2"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="12"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AH46" s="12"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AK46" s="12"/>
     </row>
     <row r="47" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
         <v>126</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="2">
-        <v>129</v>
-      </c>
-      <c r="C49" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
+        <v>129</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
         <v>255</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>62</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="55">
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="AJ5:AK5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="T23:U23"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AH6:AI6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AH6:AI6"/>
-    <mergeCell ref="AJ6:AK6"/>
     <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on Mega Code
Changed calibration messages to display on LCD instead of via serial
port.
Added process for writing to the LCD easily.
Added calibration button to PC software
</commit_message>
<xml_diff>
--- a/SMS Strings.xlsx
+++ b/SMS Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="118">
   <si>
     <t>1st</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>50 H</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>Calibrate</t>
   </si>
 </sst>
 </file>
@@ -792,7 +798,7 @@
   <dimension ref="B2:AR62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:O7"/>
+      <selection activeCell="AS23" sqref="AS23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +817,7 @@
     <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="27" width="7.140625" customWidth="1"/>
@@ -2784,29 +2790,21 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q34" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
       <c r="R34" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="T34" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="T34" s="3" t="s">
         <v>24</v>
       </c>
       <c r="U34" s="7" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="V34" s="6" t="s">
         <v>64</v>
@@ -2876,24 +2874,24 @@
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="11"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="10"/>
-      <c r="AA35" s="11"/>
-      <c r="AB35" s="10"/>
-      <c r="AC35" s="11"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="10"/>
-      <c r="AG35" s="11"/>
-      <c r="AH35" s="10"/>
-      <c r="AI35" s="11"/>
-      <c r="AJ35" s="8"/>
-      <c r="AK35" s="9"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
@@ -2908,8 +2906,12 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
+      <c r="N36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="P36" s="3" t="s">
         <v>13</v>
       </c>
@@ -3710,47 +3712,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="AJ6:AK6"/>
@@ -3765,6 +3726,47 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>